<commit_message>
Added codes in R and Python to plot agenda_1 and agenda_3
</commit_message>
<xml_diff>
--- a/data_visualization/fiscal_indicators.xlsx
+++ b/data_visualization/fiscal_indicators.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/fb59f80414e38fcc/Documentos/RA/CIUP/Policy Brief/GitHub/peruvian_policy_brief/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/fb59f80414e38fcc/Documentos/RA/CIUP/Policy Brief/GitHub/peruvian_policy_brief/data_visualization/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EC789071-F5B0-4A37-BF84-00BE4F9D85B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="19" documentId="8_{EC789071-F5B0-4A37-BF84-00BE4F9D85B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0D105880-91D0-42BC-8620-82DFA1E13953}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{F4CC1B27-4994-46CE-9DBF-DB6915EF3791}"/>
   </bookViews>
@@ -420,7 +420,7 @@
   <dimension ref="A1:C28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C28"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -444,7 +444,7 @@
         <v>-0.80633218699999998</v>
       </c>
       <c r="C2" s="1">
-        <v>-48.304279119999997</v>
+        <v>48.304279119999997</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -455,7 +455,7 @@
         <v>-0.437506387</v>
       </c>
       <c r="C3" s="1">
-        <v>-47.441048209999998</v>
+        <v>47.441048209999998</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -466,7 +466,7 @@
         <v>-5.6480740000000001E-2</v>
       </c>
       <c r="C4" s="1">
-        <v>-48.81313179</v>
+        <v>48.81313179</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -477,7 +477,7 @@
         <v>0.50813617300000002</v>
       </c>
       <c r="C5" s="1">
-        <v>-48.845082859999998</v>
+        <v>48.845082859999998</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -488,7 +488,7 @@
         <v>1.022456778</v>
       </c>
       <c r="C6" s="1">
-        <v>-44.685585770000003</v>
+        <v>44.685585770000003</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -499,7 +499,7 @@
         <v>1.7133179039999999</v>
       </c>
       <c r="C7" s="1">
-        <v>-41.848136619999998</v>
+        <v>41.848136619999998</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
@@ -510,7 +510,7 @@
         <v>4.4429424309999996</v>
       </c>
       <c r="C8" s="1">
-        <v>-33.818129620000001</v>
+        <v>33.818129620000001</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -521,7 +521,7 @@
         <v>4.9439566749999999</v>
       </c>
       <c r="C9" s="1">
-        <v>-29.57498584</v>
+        <v>29.57498584</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
@@ -532,7 +532,7 @@
         <v>4.1896231190000002</v>
       </c>
       <c r="C10" s="1">
-        <v>-26.603819640000001</v>
+        <v>26.603819640000001</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
@@ -543,7 +543,7 @@
         <v>7.3780519000000003E-2</v>
       </c>
       <c r="C11" s="1">
-        <v>-26.57796832</v>
+        <v>26.57796832</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
@@ -554,7 +554,7 @@
         <v>1.0301069060000001</v>
       </c>
       <c r="C12" s="1">
-        <v>-23.748765720000002</v>
+        <v>23.748765720000002</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
@@ -565,7 +565,7 @@
         <v>3.2594935930000002</v>
       </c>
       <c r="C13" s="1">
-        <v>-21.644469130000001</v>
+        <v>21.644469130000001</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
@@ -576,7 +576,7 @@
         <v>3.366959746</v>
       </c>
       <c r="C14" s="1">
-        <v>-19.88373868</v>
+        <v>19.88373868</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
@@ -587,7 +587,7 @@
         <v>1.9943525520000001</v>
       </c>
       <c r="C15" s="1">
-        <v>-19.15089755</v>
+        <v>19.15089755</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
@@ -598,7 +598,7 @@
         <v>0.82064914099999997</v>
       </c>
       <c r="C16" s="1">
-        <v>-19.74077003</v>
+        <v>19.74077003</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
@@ -609,7 +609,7 @@
         <v>-0.88460576899999999</v>
       </c>
       <c r="C17" s="1">
-        <v>-22.969260040000002</v>
+        <v>22.969260040000002</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
@@ -620,7 +620,7 @@
         <v>-1.247379545</v>
       </c>
       <c r="C18" s="1">
-        <v>-23.328851820000001</v>
+        <v>23.328851820000001</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
@@ -631,7 +631,7 @@
         <v>-1.780445364</v>
       </c>
       <c r="C19" s="1">
-        <v>-24.303598430000001</v>
+        <v>24.303598430000001</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
@@ -642,7 +642,7 @@
         <v>-0.937841916</v>
       </c>
       <c r="C20" s="1">
-        <v>-25.25471933</v>
+        <v>25.25471933</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
@@ -653,7 +653,7 @@
         <v>-0.239940501</v>
       </c>
       <c r="C21" s="1">
-        <v>-26.150469000000001</v>
+        <v>26.150469000000001</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
@@ -664,7 +664,7 @@
         <v>-7.1421678369999997</v>
       </c>
       <c r="C22" s="1">
-        <v>-33.950221339999999</v>
+        <v>33.950221339999999</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
@@ -675,7 +675,7 @@
         <v>-1.005318216</v>
       </c>
       <c r="C23" s="1">
-        <v>-35.309561170000002</v>
+        <v>35.309561170000002</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
@@ -686,7 +686,7 @@
         <v>-0.13465909000000001</v>
       </c>
       <c r="C24" s="1">
-        <v>-33.341152360000002</v>
+        <v>33.341152360000002</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
@@ -697,7 +697,7 @@
         <v>-1.1022459760000001</v>
       </c>
       <c r="C25" s="1">
-        <v>-32.359804089999997</v>
+        <v>32.359804089999997</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
@@ -708,7 +708,7 @@
         <v>-1.7834136869999999</v>
       </c>
       <c r="C26" s="1">
-        <v>-32.098447520000001</v>
+        <v>32.098447520000001</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
@@ -719,7 +719,7 @@
         <v>-2.5</v>
       </c>
       <c r="C27" s="1">
-        <v>-32.200000000000003</v>
+        <v>32.200000000000003</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
@@ -730,7 +730,7 @@
         <v>-2.1</v>
       </c>
       <c r="C28" s="1">
-        <v>-32.6</v>
+        <v>32.6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>